<commit_message>
add action "scroll into view" add lesson for PowerPoint 2010
</commit_message>
<xml_diff>
--- a/Document/Actions.xlsx
+++ b/Document/Actions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Action Name</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>&lt;milisecond&gt;</t>
+  </si>
+  <si>
+    <t>scroll into view</t>
+  </si>
+  <si>
+    <t>&lt;window_name&gt;|&lt;control_name(list item)&gt;</t>
   </si>
 </sst>
 </file>
@@ -119,8 +125,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Action Name" dataDxfId="0"/>
     <tableColumn id="2" name="Argument"/>
@@ -416,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,6 +482,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>